<commit_message>
Files correctly placed Again
</commit_message>
<xml_diff>
--- a/Test Cases for Raffle User Experience Page.xlsx
+++ b/Test Cases for Raffle User Experience Page.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogandhi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogandhi\Documents\GitHub\DoverInterview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8229AE-3E9C-4EC9-AC1A-1D482612B0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C7274A-7A58-458E-9529-256BF066AFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="20" windowWidth="19170" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>User Should be able to Navigate to URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Should be able to Enter credentials </t>
   </si>
   <si>
     <t>On Clicking Submit button Form should be submitted and number of Raffle registered</t>
@@ -284,12 +281,6 @@
     <t>Enter a name field should have border in Blue</t>
   </si>
   <si>
-    <t>User should able to blue border as per design document</t>
-  </si>
-  <si>
-    <t>User should be able to see black border and not blue</t>
-  </si>
-  <si>
     <t>Defect to be added</t>
   </si>
   <si>
@@ -331,6 +322,18 @@
   </si>
   <si>
     <t>Defect - Added Defect ID 001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Should be add alpha numerical text </t>
+  </si>
+  <si>
+    <t>User is able to enter alpha Numberical text in Text Field</t>
+  </si>
+  <si>
+    <t>User is not able to see blue border and a  black border is seen</t>
+  </si>
+  <si>
+    <t>User should able to view blue border as per design document</t>
   </si>
 </sst>
 </file>
@@ -400,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -426,9 +429,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="64" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,7 +767,7 @@
         <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -781,13 +781,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
@@ -799,7 +799,7 @@
         <v>17</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K2" s="6"/>
     </row>
@@ -814,13 +814,13 @@
         <v>2</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="6"/>
     </row>
@@ -838,13 +838,13 @@
         <v>16</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -852,19 +852,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
@@ -876,7 +876,7 @@
         <v>17</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -894,10 +894,10 @@
         <v>15</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -915,13 +915,13 @@
         <v>16</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
@@ -929,19 +929,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
@@ -953,7 +953,7 @@
         <v>17</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -971,14 +971,14 @@
         <v>15</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
@@ -992,13 +992,13 @@
         <v>16</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="87" x14ac:dyDescent="0.35">
@@ -1006,19 +1006,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G11" s="9">
         <v>1</v>
@@ -1030,7 +1030,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K11" s="6"/>
     </row>
@@ -1048,16 +1048,16 @@
         <v>15</v>
       </c>
       <c r="I12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="L12" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -1078,19 +1078,19 @@
         <v>5</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="9">
         <v>1</v>
@@ -1102,7 +1102,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K14" s="6"/>
     </row>
@@ -1117,13 +1117,13 @@
         <v>2</v>
       </c>
       <c r="H15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="J15" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -1138,16 +1138,16 @@
         <v>3</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="J16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="K16" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
@@ -1155,19 +1155,19 @@
         <v>6</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="9">
         <v>1</v>
@@ -1179,11 +1179,11 @@
         <v>17</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
@@ -1194,16 +1194,16 @@
         <v>2</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
@@ -1211,19 +1211,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
@@ -1235,11 +1235,11 @@
         <v>17</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
@@ -1250,17 +1250,17 @@
         <v>2</v>
       </c>
       <c r="H20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="J20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
@@ -1271,16 +1271,16 @@
         <v>3</v>
       </c>
       <c r="H21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="K21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1288,19 +1288,19 @@
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G22" s="9">
         <v>1</v>
@@ -1312,7 +1312,7 @@
         <v>17</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -1327,19 +1327,19 @@
         <v>2</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>88</v>
+        <v>24</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1347,19 +1347,19 @@
         <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G24" s="9">
         <v>1</v>
@@ -1371,11 +1371,11 @@
         <v>17</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
@@ -1386,13 +1386,13 @@
         <v>2</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -1407,19 +1407,19 @@
         <v>3</v>
       </c>
       <c r="H26" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I26" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="J26" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>77</v>
+        <v>33</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="58" x14ac:dyDescent="0.35">
@@ -1427,19 +1427,19 @@
         <v>10</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G27" s="9">
         <v>1</v>
@@ -1451,11 +1451,11 @@
         <v>17</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="5"/>
@@ -1466,19 +1466,19 @@
         <v>2</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L28" s="11" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>